<commit_message>
update kpay config to payment channel
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Kpay/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Portal_Kpay/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Kpay\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8AD2CA-0CFB-473B-A30D-D495FAA19B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC91E999-8A9E-45BA-91F9-307401AC89A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="1932" windowWidth="21588" windowHeight="10644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -203,9 +203,6 @@
     <t>RPA_Moon_Cred_Gmail</t>
   </si>
   <si>
-    <t>RPA_Moon_SheetIdConfig_Transport</t>
-  </si>
-  <si>
     <t>RPA_Moon_PathMasterFolder</t>
   </si>
   <si>
@@ -222,6 +219,9 @@
   </si>
   <si>
     <t>RPA_Moon_UploadBucket</t>
+  </si>
+  <si>
+    <t>RPA_Moon_SheetIdConfig</t>
   </si>
 </sst>
 </file>
@@ -651,7 +651,7 @@
         <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -2910,7 +2910,7 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -2918,7 +2918,7 @@
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -2926,7 +2926,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -2934,7 +2934,7 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -2942,7 +2942,7 @@
         <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -2950,7 +2950,7 @@
         <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>